<commit_message>
notebook modified to include method that uses only opencv
</commit_message>
<xml_diff>
--- a/notebooks/output.xlsx
+++ b/notebooks/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,70 +424,265 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Date collected|Plot__|Species |Sex Weight</t>
+          <t>Date collected</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Plot__</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Species</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Sex Weight</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1/9/78 1|DM M 40</t>
+          <t>1/9/78</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DM</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>40</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1/9/78 1|DM EF 36</t>
+          <t>1/9/78</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>DM</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>EF</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>36</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1/9/78 41|DS EF 135</t>
+          <t>1/9/78</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>EF</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>135</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1/20/78 1|DM F 39</t>
+          <t>1/20/78</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>DM</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>39</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1/20/78 2|DM M 43</t>
+          <t>1/20/78</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>DM</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>43</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1/20/78 2|DS EF 144</t>
+          <t>1/20/78</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>EF</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>144</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3/13/78 2|DM EF 51</t>
+          <t>3/13/78</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>DM</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>EF</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>51</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3/13/78 2|DM EF 44</t>
+          <t>3/13/78</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>DM</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>EF</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>44</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3/13/78 2|DS EF 146</t>
+          <t>3/13/78</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>EF</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>146</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ocr using only OpenCV
</commit_message>
<xml_diff>
--- a/notebooks/output.xlsx
+++ b/notebooks/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,269 +422,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Date collected</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Plot__</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Sex Weight</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1/9/78</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>DM</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1/9/78</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>DM</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>EF</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1/9/78</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>DS</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>EF</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>135</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1/20/78</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>DM</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1/20/78</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>DM</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1/20/78</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>DS</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>EF</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>144</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>3/13/78</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>DM</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>EF</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>3/13/78</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>DM</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>EF</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>3/13/78</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>DS</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>EF</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>146</t>
-        </is>
-      </c>
+      <c r="A1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>